<commit_message>
Remove enumeration in graph
</commit_message>
<xml_diff>
--- a/input_data/data_errors/5_composicao/composicao.xlsx
+++ b/input_data/data_errors/5_composicao/composicao.xlsx
@@ -950,10 +950,18 @@
       <c r="X14" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+      <c r="A15" s="4">
+        <v>77</v>
+      </c>
+      <c r="B15" s="4">
+        <v>55</v>
+      </c>
+      <c r="C15" s="5">
+        <v>6</v>
+      </c>
+      <c r="D15" s="5">
+        <v>7</v>
+      </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -976,10 +984,18 @@
       <c r="X15" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
+      <c r="A16" s="4">
+        <v>77</v>
+      </c>
+      <c r="B16" s="4">
+        <v>66</v>
+      </c>
+      <c r="C16" s="5">
+        <v>6</v>
+      </c>
+      <c r="D16" s="5">
+        <v>7</v>
+      </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>

</xml_diff>

<commit_message>
close #3: Verify if the hierarchy is a tree
</commit_message>
<xml_diff>
--- a/input_data/data_errors/5_composicao/composicao.xlsx
+++ b/input_data/data_errors/5_composicao/composicao.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>codigo_pai</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>nivel_filho</t>
+  </si>
+  <si>
+    <t>php</t>
   </si>
 </sst>
 </file>
@@ -515,7 +518,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="5">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="D2" s="5">
         <v>1</v>
@@ -684,8 +687,8 @@
       <c r="B7" s="4">
         <v>5004</v>
       </c>
-      <c r="C7" s="5">
-        <v>3</v>
+      <c r="C7" s="5" t="s">
+        <v>4</v>
       </c>
       <c r="D7" s="5">
         <v>4</v>

</xml_diff>

<commit_message>
close #76: Add minimum value check for indicator IDs
</commit_message>
<xml_diff>
--- a/input_data/data_errors/5_composicao/composicao.xlsx
+++ b/input_data/data_errors/5_composicao/composicao.xlsx
@@ -862,10 +862,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="4">
-        <v>5033</v>
+        <v>-88</v>
       </c>
       <c r="B14" s="4">
-        <v>5013</v>
+        <v>-89</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -1132,7 +1132,7 @@
       <c r="W23" s="3"/>
       <c r="X23" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="5"/>
@@ -1158,7 +1158,7 @@
       <c r="W24" s="3"/>
       <c r="X24" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="5"/>
@@ -1184,7 +1184,7 @@
       <c r="W25" s="3"/>
       <c r="X25" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="5"/>
@@ -1210,7 +1210,7 @@
       <c r="W26" s="3"/>
       <c r="X26" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="5"/>

</xml_diff>